<commit_message>
Updated Stack vs Queue tests in xlsx.
</commit_message>
<xml_diff>
--- a/Test Results.xlsx
+++ b/Test Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CSC3095-Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB94F82-B9A2-4217-B8A9-55F972726A25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DC05E3-94AC-4682-AA2C-153E8CE541C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{43AB4C6B-370F-4888-996C-F8629A52645F}"/>
+    <workbookView minimized="1" xWindow="9600" yWindow="3360" windowWidth="28800" windowHeight="15435" xr2:uid="{43AB4C6B-370F-4888-996C-F8629A52645F}"/>
   </bookViews>
   <sheets>
     <sheet name="Speed Tests" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="30">
   <si>
     <t>Span Fill</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Queue</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -419,6 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2198,6 +2202,638 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
+              <a:t>Town</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Speed - Pixel per second (p*s^-6)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Speed Tests'!$A$93</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stack</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Speed Tests'!$C$84:$G$84</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Four Way (Recursive)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Four Way (Linear)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Span Fill</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Walk Based</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Speed Tests'!$C$93:$G$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.45621037802301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4119511622446583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51350082178915235</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.369570321671754</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6535571730453158</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-46F7-479C-B27E-64C2ECB8F1D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Speed Tests'!$A$94</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Queue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Speed Tests'!$C$84:$G$84</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Four Way (Recursive)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Four Way (Linear)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Span Fill</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Walk Based</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Speed Tests'!$C$94:$G$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.5039915473115755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.522657900915708</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53146278469124208</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.471002582765907</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8014792204742898</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-46F7-479C-B27E-64C2ECB8F1D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="554097808"/>
+        <c:axId val="554096496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="554097808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554096496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="554096496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Pixels per microsecond (p*s-^6</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554097808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
               <a:t>Square Size</a:t>
             </a:r>
           </a:p>
@@ -3939,7 +4575,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5712,7 +6348,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7397,7 +8033,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -9320,10 +9956,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Speed Tests'!$A$5:$A$20</c:f>
+              <c:f>'Speed Tests'!$A$5:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -9347,40 +9983,16 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Speed Tests'!$C$5:$C$20</c:f>
+              <c:f>'Speed Tests'!$C$5:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -9404,30 +10016,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3680</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9819,6 +10407,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Speed Tests'!$A$5:$A$20</c:f>
@@ -10217,6 +10820,22 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="7"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10398,31 +11017,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Speed Tests'!$C$45:$J$45</c:f>
+              <c:f>'Speed Tests'!$C$45:$L$45</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Four Way (Recursive)</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Four Way (Linear)</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Span Fill</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Walk Based</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Four Way (Recursive)</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Four Way (Linear)</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Span Fill</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Walk Based</c:v>
                 </c:pt>
               </c:strCache>
@@ -10430,32 +11055,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Speed Tests'!$C$46:$J$46</c:f>
+              <c:f>'Speed Tests'!$C$46:$L$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1.4583025050206109</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.4387176964429462</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.33687301259295122</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2.8075095071693155</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1.5455025895782686</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1.4581545759324428</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.35147071976905209</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>2.7496861785959918</c:v>
                 </c:pt>
               </c:numCache>
@@ -10493,31 +11124,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Speed Tests'!$C$45:$J$45</c:f>
+              <c:f>'Speed Tests'!$C$45:$L$45</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Four Way (Recursive)</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Four Way (Linear)</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Span Fill</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Walk Based</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Four Way (Recursive)</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Four Way (Linear)</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Span Fill</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Walk Based</c:v>
                 </c:pt>
               </c:strCache>
@@ -10525,32 +11162,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Speed Tests'!$C$47:$J$47</c:f>
+              <c:f>'Speed Tests'!$C$47:$L$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1.467607843137255</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.3746501060284761</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.33786610118146015</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2.7291875189336565</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1.6746666666666667</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1.4855789154801577</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.33868039987882459</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>2.6922144804604664</c:v>
                 </c:pt>
               </c:numCache>
@@ -10588,31 +11231,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Speed Tests'!$C$45:$J$45</c:f>
+              <c:f>'Speed Tests'!$C$45:$L$45</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Four Way (Recursive)</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Four Way (Linear)</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Span Fill</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Walk Based</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Four Way (Recursive)</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Four Way (Linear)</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Span Fill</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Walk Based</c:v>
                 </c:pt>
               </c:strCache>
@@ -10620,32 +11269,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Speed Tests'!$C$48:$J$48</c:f>
+              <c:f>'Speed Tests'!$C$48:$L$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>1.6535571730453158</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1.45621037802301</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.4119511622446583</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.51350082178915235</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>13.369570321671754</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>1.8014792204742898</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1.5039915473115755</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1.522657900915708</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.53146278469124208</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>13.471002582765907</c:v>
                 </c:pt>
               </c:numCache>
@@ -10654,6 +11309,220 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-56C8-47C3-93DD-8C28E1259749}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Speed Tests'!$A$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>25% Checkered</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Speed Tests'!$C$45:$L$45</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Four Way (Recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Four Way (Linear)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Span Fill</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Walk Based</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Four Way (Recursive)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Four Way (Linear)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Span Fill</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Walk Based</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Speed Tests'!$C$49:$L$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.2217881944444444</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9709201388888888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5933159722222223</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3732638888888888</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.686197916666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2829861111111112</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0698784722222223</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6024305555555554</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3216145833333335</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.8472222222222223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-37E6-4FEF-A648-B739BC8181DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Speed Tests'!$A$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50% Checkered</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Speed Tests'!$C$45:$L$45</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Four Way (Recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Four Way (Linear)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Span Fill</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Walk Based</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Four Way (Recursive)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Four Way (Linear)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Span Fill</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Walk Based</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Speed Tests'!$C$50:$L$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.74276315789473679</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0427631578947367</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5271929824561403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3642543859649123</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2635964912280704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.70197368421052631</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9089912280701755</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4978070175438596</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1173245614035086</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.117105263157895</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-37E6-4FEF-A648-B739BC8181DB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12574,6 +13443,18 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="8"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="9"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="10"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15487,557 +16368,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Practise</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Town 100x100</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Speed Tests'!$B$40:$L$40</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>No. Pixels</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Brute Force</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Four Way (Recursive)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Four Way (Linear)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Span Fill</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Walk Based</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Brute Force</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Four Way (Recursive)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Four Way (Linear)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Span Fill</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Walk Based</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Speed Tests'!$B$41:$L$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>8518</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14085</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12404</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12027</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4374</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>113882</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>15345</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12811</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12970</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4527</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>114746</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-16CE-4C5F-B93B-C78BB9E98B7B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Speed Tests'!$B$40:$L$40</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>No. Pixels</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Brute Force</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Four Way (Recursive)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Four Way (Linear)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Span Fill</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Walk Based</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Brute Force</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Four Way (Recursive)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Four Way (Linear)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Span Fill</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Walk Based</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Speed Tests'!$B$42:$L$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2304</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2815</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4541</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5975</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5468</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>17709</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2956</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4769</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5349</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>13472</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-16CE-4C5F-B93B-C78BB9E98B7B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Speed Tests'!$B$40:$L$40</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>No. Pixels</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Brute Force</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Four Way (Recursive)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Four Way (Linear)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Span Fill</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Walk Based</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Brute Force</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Four Way (Recursive)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Four Way (Linear)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Span Fill</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Walk Based</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Speed Tests'!$B$43:$L$43</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>4560</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3387</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9315</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11524</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10781</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19442</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3201</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8705</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11390</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9655</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>18774</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-16CE-4C5F-B93B-C78BB9E98B7B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="554757192"/>
-        <c:axId val="554756864"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="554757192"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="554756864"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="554756864"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="554757192"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
               <a:t>Circle</a:t>
             </a:r>
             <a:r>
@@ -16168,9 +16498,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Speed Tests'!$C$84:$F$84</c:f>
+              <c:f>'Speed Tests'!$C$84:$G$84</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Four Way (Recursive)</c:v>
                 </c:pt>
@@ -16182,16 +16512,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Walk Based</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Brute Force</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Speed Tests'!$C$85:$F$85</c:f>
+              <c:f>'Speed Tests'!$C$85:$G$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1.4583025050206109</c:v>
                 </c:pt>
@@ -16203,6 +16536,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.8075095071693155</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79181689484901108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16297,9 +16633,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Speed Tests'!$C$84:$F$84</c:f>
+              <c:f>'Speed Tests'!$C$84:$G$84</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Four Way (Recursive)</c:v>
                 </c:pt>
@@ -16311,16 +16647,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Walk Based</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Brute Force</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Speed Tests'!$C$86:$F$86</c:f>
+              <c:f>'Speed Tests'!$C$86:$G$86</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1.5455025895782686</c:v>
                 </c:pt>
@@ -16332,6 +16671,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.7496861785959918</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81647275822928489</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16339,6 +16681,553 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DE76-4C05-9057-AF62F2EFD271}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="554097808"/>
+        <c:axId val="554096496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="554097808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554096496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="554096496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554097808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Square</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Speed - Pixel per second (p*s^-6)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Speed Tests'!$A$89</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stack</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Speed Tests'!$C$84:$G$84</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Four Way (Recursive)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Four Way (Linear)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Span Fill</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Walk Based</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Speed Tests'!$C$89:$G$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.467607843137255</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3746501060284761</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33786610118146015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7291875189336565</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.69143411087549222</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4550-48F0-B28C-CFF3B3D84635}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Speed Tests'!$A$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Queue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Speed Tests'!$C$84:$G$84</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Four Way (Recursive)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Four Way (Linear)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Span Fill</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Walk Based</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Brute Force</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Speed Tests'!$C$90:$G$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.6746666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4855789154801577</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33868039987882459</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6922144804604664</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67194668282338688</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4550-48F0-B28C-CFF3B3D84635}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -16738,6 +17627,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -17575,7 +18504,7 @@
 </file>
 
 <file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -17602,8 +18531,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -17704,6 +18633,509 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -18090,7 +19522,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18606,7 +20038,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -19122,7 +20554,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -22698,7 +24130,7 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -22902,23 +24334,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -23023,8 +24454,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -23156,20 +24587,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -23747,8 +25177,8 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>178253</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>65314</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>448235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
@@ -23783,16 +25213,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>550408</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>57831</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>90967</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>113860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>242888</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>25174</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>336176</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23897,12 +25327,12 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>87558</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>16921</xdr:rowOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>369167</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>93121</xdr:rowOff>
     </xdr:to>
@@ -23931,23 +25361,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>102053</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>125186</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>662667</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>132869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>170088</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>119743</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1152524</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>64834</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1156116-CB7F-4E3C-B14D-580A5AB1D77B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7197E792-421F-46BD-AFD0-BDF423707CEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23967,23 +25397,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>662667</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>54428</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>56830</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>165687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1152524</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>353785</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>67715</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7197E792-421F-46BD-AFD0-BDF423707CEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E5B83D5-A8C9-415D-BA4C-844EEB8E008A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24003,27 +25433,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>68035</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>291353</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>353785</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>78921</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>588308</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>92528</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="15" name="Chart 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E5B83D5-A8C9-415D-BA4C-844EEB8E008A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{374DA74B-8A73-474E-B72B-5A130C806A54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -24032,6 +25464,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>280147</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>577102</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>114940</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B10021B-076B-491F-B64B-0CA9E462001D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -24494,10 +25964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AD4CD4-0469-4BD9-B9A9-48BE844E1797}">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25805,27 +27275,33 @@
         <v>8</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="E45" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="F45" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="G45" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="H45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="10" t="s">
+      <c r="J45" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I45" s="10" t="s">
+      <c r="K45" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="J45" s="10" t="s">
+      <c r="L45" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -25837,36 +27313,42 @@
         <f>SUM(B23:B38)</f>
         <v>324229</v>
       </c>
-      <c r="C46" s="21">
+      <c r="C46" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="21">
         <f>SUM(SUM(C23:C31)/SUM(B23:B31))</f>
         <v>1.4583025050206109</v>
       </c>
-      <c r="D46" s="10" cm="1">
-        <f t="array" ref="D46">SUM(D23:D38/$B46)</f>
+      <c r="E46" s="10" cm="1">
+        <f t="array" ref="E46">SUM(D23:D38/$B46)</f>
         <v>1.4387176964429462</v>
       </c>
-      <c r="E46" s="10" cm="1">
-        <f t="array" ref="E46">SUM(E23:E38/$B46)</f>
+      <c r="F46" s="10" cm="1">
+        <f t="array" ref="F46">SUM(E23:E38/$B46)</f>
         <v>0.33687301259295122</v>
       </c>
-      <c r="F46" s="10" cm="1">
-        <f t="array" ref="F46">SUM(F23:F38/$B46)</f>
+      <c r="G46" s="10" cm="1">
+        <f t="array" ref="G46">SUM(F23:F38/$B46)</f>
         <v>2.8075095071693155</v>
       </c>
-      <c r="G46">
+      <c r="H46" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I46">
         <f>SUM(SUM(G23:G31)/SUM(B23:B31))</f>
         <v>1.5455025895782686</v>
       </c>
-      <c r="H46" s="10" cm="1">
-        <f t="array" ref="H46">SUM(H23:H38/$B46)</f>
+      <c r="J46" s="10" cm="1">
+        <f t="array" ref="J46">SUM(H23:H38/$B46)</f>
         <v>1.4581545759324428</v>
       </c>
-      <c r="I46" s="4" cm="1">
-        <f t="array" ref="I46">SUM(I23:I38/$B46)</f>
+      <c r="K46" s="10" cm="1">
+        <f t="array" ref="K46">SUM(I23:I38/$B46)</f>
         <v>0.35147071976905209</v>
       </c>
-      <c r="J46" s="10" cm="1">
-        <f t="array" ref="J46">SUM(J23:J38/$B46)</f>
+      <c r="L46" s="10" cm="1">
+        <f t="array" ref="L46">SUM(J23:J38/$B46)</f>
         <v>2.7496861785959918</v>
       </c>
     </row>
@@ -25878,36 +27360,42 @@
         <f>SUM(B5:B20)</f>
         <v>412625</v>
       </c>
-      <c r="C47" s="23">
+      <c r="C47" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="23">
         <f>SUM(SUM(C5:C12)/SUM(B5:B12))</f>
         <v>1.467607843137255</v>
       </c>
-      <c r="D47" s="11" cm="1">
-        <f t="array" ref="D47">SUM(D5:D20/$B47)</f>
+      <c r="E47" s="11" cm="1">
+        <f t="array" ref="E47">SUM(D5:D20/$B47)</f>
         <v>1.3746501060284761</v>
       </c>
-      <c r="E47" s="11" cm="1">
-        <f t="array" ref="E47">SUM(E5:E20/$B47)</f>
+      <c r="F47" s="11" cm="1">
+        <f t="array" ref="F47">SUM(E5:E20/$B47)</f>
         <v>0.33786610118146015</v>
       </c>
-      <c r="F47" s="11" cm="1">
-        <f t="array" ref="F47">SUM(F5:F20/$B47)</f>
+      <c r="G47" s="11" cm="1">
+        <f t="array" ref="G47">SUM(F5:F20/$B47)</f>
         <v>2.7291875189336565</v>
       </c>
-      <c r="G47">
+      <c r="H47" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I47">
         <f>SUM(SUM(G5:G12)/SUM(B5:B12))</f>
         <v>1.6746666666666667</v>
       </c>
-      <c r="H47" s="11" cm="1">
-        <f t="array" ref="H47">SUM(H5:H20/$B47)</f>
+      <c r="J47" s="11" cm="1">
+        <f t="array" ref="J47">SUM(H5:H20/$B47)</f>
         <v>1.4855789154801577</v>
       </c>
-      <c r="I47" s="5" cm="1">
-        <f t="array" ref="I47">SUM(I5:I20/$B47)</f>
+      <c r="K47" s="11" cm="1">
+        <f t="array" ref="K47">SUM(I5:I20/$B47)</f>
         <v>0.33868039987882459</v>
       </c>
-      <c r="J47" s="11" cm="1">
-        <f t="array" ref="J47">SUM(J5:J20/$B47)</f>
+      <c r="L47" s="11" cm="1">
+        <f t="array" ref="L47">SUM(J5:J20/$B47)</f>
         <v>2.6922144804604664</v>
       </c>
     </row>
@@ -25919,44 +27407,148 @@
         <v>8518</v>
       </c>
       <c r="C48" s="20">
+        <f>SUM(C41/B48)</f>
+        <v>1.6535571730453158</v>
+      </c>
+      <c r="D48" s="20">
         <f>SUM(D41/B48)</f>
         <v>1.45621037802301</v>
       </c>
-      <c r="D48" s="12">
+      <c r="E48" s="20">
         <f>SUM(E41/B48)</f>
         <v>1.4119511622446583</v>
       </c>
-      <c r="E48" s="12">
+      <c r="F48" s="20">
         <f>SUM(F41/B48)</f>
         <v>0.51350082178915235</v>
       </c>
-      <c r="F48" s="12">
+      <c r="G48" s="20">
         <f>SUM(G41/B48)</f>
         <v>13.369570321671754</v>
       </c>
-      <c r="G48" s="12">
+      <c r="H48" s="12">
+        <f>SUM(H41/B48)</f>
+        <v>1.8014792204742898</v>
+      </c>
+      <c r="I48" s="20">
         <f>SUM(I41/B48)</f>
         <v>1.5039915473115755</v>
       </c>
-      <c r="H48" s="12">
+      <c r="J48" s="20">
         <f>SUM(J41/B48)</f>
         <v>1.522657900915708</v>
       </c>
-      <c r="I48" s="7">
+      <c r="K48" s="20">
         <f>SUM(K41/B48)</f>
         <v>0.53146278469124208</v>
       </c>
-      <c r="J48" s="12">
+      <c r="L48" s="20">
         <f>SUM(L41/B48)</f>
         <v>13.471002582765907</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="17">
+        <v>2304</v>
+      </c>
+      <c r="C49" s="20">
+        <f>SUM(C42/B49)</f>
+        <v>1.2217881944444444</v>
+      </c>
+      <c r="D49" s="20">
+        <f>SUM(D42/B49)</f>
+        <v>1.9709201388888888</v>
+      </c>
+      <c r="E49" s="20">
+        <f t="shared" ref="E49:E50" si="2">SUM(E42/B49)</f>
+        <v>2.5933159722222223</v>
+      </c>
+      <c r="F49" s="20">
+        <f t="shared" ref="F49:F50" si="3">SUM(F42/B49)</f>
+        <v>2.3732638888888888</v>
+      </c>
+      <c r="G49" s="20">
+        <f t="shared" ref="G49:G50" si="4">SUM(G42/B49)</f>
+        <v>7.686197916666667</v>
+      </c>
+      <c r="H49" s="12">
+        <f t="shared" ref="H49:H50" si="5">SUM(H42/B49)</f>
+        <v>1.2829861111111112</v>
+      </c>
+      <c r="I49" s="20">
+        <f t="shared" ref="I49:I50" si="6">SUM(I42/B49)</f>
+        <v>2.0698784722222223</v>
+      </c>
+      <c r="J49" s="20">
+        <f t="shared" ref="J49:J50" si="7">SUM(J42/B49)</f>
+        <v>2.6024305555555554</v>
+      </c>
+      <c r="K49" s="20">
+        <f>SUM(K42/B49)</f>
+        <v>2.3216145833333335</v>
+      </c>
+      <c r="L49" s="20">
+        <f t="shared" ref="L49:L50" si="8">SUM(L42/B49)</f>
+        <v>5.8472222222222223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="16">
+        <v>4560</v>
+      </c>
+      <c r="C50" s="20">
+        <f>SUM(C43/B50)</f>
+        <v>0.74276315789473679</v>
+      </c>
+      <c r="D50" s="20">
+        <f t="shared" ref="D50" si="9">SUM(D43/B50)</f>
+        <v>2.0427631578947367</v>
+      </c>
+      <c r="E50" s="20">
+        <f t="shared" si="2"/>
+        <v>2.5271929824561403</v>
+      </c>
+      <c r="F50" s="20">
+        <f t="shared" si="3"/>
+        <v>2.3642543859649123</v>
+      </c>
+      <c r="G50" s="20">
+        <f t="shared" si="4"/>
+        <v>4.2635964912280704</v>
+      </c>
+      <c r="H50" s="12">
+        <f t="shared" si="5"/>
+        <v>0.70197368421052631</v>
+      </c>
+      <c r="I50" s="20">
+        <f t="shared" si="6"/>
+        <v>1.9089912280701755</v>
+      </c>
+      <c r="J50" s="20">
+        <f t="shared" si="7"/>
+        <v>2.4978070175438596</v>
+      </c>
+      <c r="K50" s="20">
+        <f t="shared" ref="K50" si="10">SUM(K43/B50)</f>
+        <v>2.1173245614035086</v>
+      </c>
+      <c r="L50" s="20">
+        <f t="shared" si="8"/>
+        <v>4.117105263157895</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A52" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
@@ -25985,7 +27577,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>5</v>
       </c>
@@ -26017,12 +27609,12 @@
         <v>5.9869719564344733E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <v>75</v>
       </c>
       <c r="B55" s="11">
-        <f t="shared" ref="B55" si="2">SUM(A55 * 4 - 4)</f>
+        <f t="shared" ref="B55" si="11">SUM(A55 * 4 - 4)</f>
         <v>296</v>
       </c>
       <c r="C55" s="11">
@@ -26049,12 +27641,12 @@
         <v>2.1479045215075407E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>400</v>
       </c>
       <c r="B56" s="12">
-        <f t="shared" ref="B56" si="3">SUM(A56 * 4 - 4)</f>
+        <f t="shared" ref="B56" si="12">SUM(A56 * 4 - 4)</f>
         <v>1596</v>
       </c>
       <c r="C56" s="12">
@@ -26075,7 +27667,7 @@
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -26083,7 +27675,7 @@
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>23</v>
       </c>
@@ -26093,7 +27685,7 @@
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="10" t="s">
         <v>20</v>
@@ -26120,7 +27712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>21</v>
       </c>
@@ -26155,7 +27747,7 @@
         <v>891528</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>7</v>
       </c>
@@ -26190,7 +27782,7 @@
         <v>1110875</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -26198,7 +27790,7 @@
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -26206,7 +27798,7 @@
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -26249,7 +27841,9 @@
       <c r="F84" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G84" s="6"/>
+      <c r="G84" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
       <c r="J84" s="6"/>
@@ -26278,6 +27872,10 @@
         <f t="array" ref="F85">SUM(F23:F38/$B85)</f>
         <v>2.8075095071693155</v>
       </c>
+      <c r="G85" s="10">
+        <f>SUM(B60/$B85)</f>
+        <v>0.79181689484901108</v>
+      </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
@@ -26302,6 +27900,172 @@
       <c r="F86" s="3" cm="1">
         <f t="array" ref="F86">SUM(J23:J38/$B85)</f>
         <v>2.7496861785959918</v>
+      </c>
+      <c r="G86" s="10">
+        <f>SUM(F60/$B86)</f>
+        <v>0.81647275822928489</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F88" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G88" s="28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>27</v>
+      </c>
+      <c r="B89" s="10">
+        <f>SUM(B5:B20)</f>
+        <v>412625</v>
+      </c>
+      <c r="C89" s="21">
+        <f>SUM(SUM(C5:C12)/SUM(B5:B12))</f>
+        <v>1.467607843137255</v>
+      </c>
+      <c r="D89" s="11" cm="1">
+        <f t="array" ref="D89">SUM(D5:D20/$B89)</f>
+        <v>1.3746501060284761</v>
+      </c>
+      <c r="E89" s="11" cm="1">
+        <f t="array" ref="E89">SUM(E5:E20/$B89)</f>
+        <v>0.33786610118146015</v>
+      </c>
+      <c r="F89" s="11" cm="1">
+        <f t="array" ref="F89">SUM(F5:F20/$B89)</f>
+        <v>2.7291875189336565</v>
+      </c>
+      <c r="G89" s="10">
+        <f>SUM(B61/$B89)</f>
+        <v>0.69143411087549222</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B90" s="3">
+        <f>SUM(B5:B20)</f>
+        <v>412625</v>
+      </c>
+      <c r="C90" s="8">
+        <f>SUM(SUM(G5:G12)/SUM(B5:B12))</f>
+        <v>1.6746666666666667</v>
+      </c>
+      <c r="D90" s="12" cm="1">
+        <f t="array" ref="D90">SUM(H5:H20/$B90)</f>
+        <v>1.4855789154801577</v>
+      </c>
+      <c r="E90" s="12" cm="1">
+        <f t="array" ref="E90">SUM(I5:I20/$B90)</f>
+        <v>0.33868039987882459</v>
+      </c>
+      <c r="F90" s="12" cm="1">
+        <f t="array" ref="F90">SUM(J5:J20/$B90)</f>
+        <v>2.6922144804604664</v>
+      </c>
+      <c r="G90" s="3">
+        <f>SUM(F61/$B90)</f>
+        <v>0.67194668282338688</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F92" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G92" s="28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93" s="10">
+        <f>SUM(B48)</f>
+        <v>8518</v>
+      </c>
+      <c r="C93" s="21">
+        <f>D48</f>
+        <v>1.45621037802301</v>
+      </c>
+      <c r="D93" s="21">
+        <f t="shared" ref="D93:F93" si="13">E48</f>
+        <v>1.4119511622446583</v>
+      </c>
+      <c r="E93" s="21">
+        <f t="shared" si="13"/>
+        <v>0.51350082178915235</v>
+      </c>
+      <c r="F93" s="21">
+        <f t="shared" si="13"/>
+        <v>13.369570321671754</v>
+      </c>
+      <c r="G93" s="10">
+        <f>C48</f>
+        <v>1.6535571730453158</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94" s="3">
+        <f>SUM(B9:B24)</f>
+        <v>411976</v>
+      </c>
+      <c r="C94" s="21">
+        <f>I48</f>
+        <v>1.5039915473115755</v>
+      </c>
+      <c r="D94" s="21">
+        <f t="shared" ref="D94:G94" si="14">J48</f>
+        <v>1.522657900915708</v>
+      </c>
+      <c r="E94" s="21">
+        <f t="shared" si="14"/>
+        <v>0.53146278469124208</v>
+      </c>
+      <c r="F94" s="21">
+        <f t="shared" si="14"/>
+        <v>13.471002582765907</v>
+      </c>
+      <c r="G94" s="21">
+        <f>H48</f>
+        <v>1.8014792204742898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>